<commit_message>
update localization csv and ColorCode
please let me know if you understand the colorcode summary
</commit_message>
<xml_diff>
--- a/ROOT_demo/Assets/Localization.xlsx
+++ b/ROOT_demo/Assets/Localization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_theArchitect\A-Game Works\R.O.O.T\R.O.O.T_Unity\ROOT_demo\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuxuan\Documents\Git\R.O.O.T_Unity\ROOT_demo\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98655292-77AB-4D97-984A-02D25AFC9A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8F3B7B-7305-4627-B296-7567A65E090B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1450" yWindow="2460" windowWidth="18400" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="1" r:id="rId1"/>
@@ -49,429 +49,460 @@
     <t>BasicControl_KM</t>
   </si>
   <si>
-    <t>【方向键】：移动光标
+    <t>BasicControl_Touch</t>
+  </si>
+  <si>
+    <t>CareerButton</t>
+  </si>
+  <si>
+    <t>生涯模式</t>
+  </si>
+  <si>
+    <t>Career</t>
+  </si>
+  <si>
+    <t>EndingMessageNormal_EarnedMoney</t>
+  </si>
+  <si>
+    <t>时间到了，你赚了{[VALUE]}块钱[i2p_Zero]时间到了，但你没赚钱</t>
+  </si>
+  <si>
+    <t>Time Up, and you earned {[VALUE]} money[i2p_Zero]Time Up, and you earned no money</t>
+  </si>
+  <si>
+    <t>EndingMessageNormal_NoEarnedMoney</t>
+  </si>
+  <si>
+    <t>时间到了，你赔了{[VALUE]}块钱[i2p_Zero]时间到了，但你也没赔钱</t>
+  </si>
+  <si>
+    <t>Time Up, and you lost {[VALUE]} money[i2p_Zero]Time Up, but you haven't lost money</t>
+  </si>
+  <si>
+    <t>EndingMessageNormal_NoMoney</t>
+  </si>
+  <si>
+    <t>你没钱了！</t>
+  </si>
+  <si>
+    <t>You've run out of money.</t>
+  </si>
+  <si>
+    <t>EndingMessageTutorial</t>
+  </si>
+  <si>
+    <t>本节教程结束~</t>
+  </si>
+  <si>
+    <t>This section of tutorial has concluded</t>
+  </si>
+  <si>
+    <t>GameOver</t>
+  </si>
+  <si>
+    <t>游戏结束</t>
+  </si>
+  <si>
+    <t>GAME OVER</t>
+  </si>
+  <si>
+    <t>HForHint_KM</t>
+  </si>
+  <si>
+    <t>按住&lt;b&gt;[H]&lt;/b&gt;键查看操作说明</t>
+  </si>
+  <si>
+    <t>Hold &lt;b&gt;[H]&lt;/b&gt; for controlling</t>
+  </si>
+  <si>
+    <t>HForHint_Touch</t>
+  </si>
+  <si>
+    <t>按住这里查看操作说明</t>
+  </si>
+  <si>
+    <t>Hold Here for Hint</t>
+  </si>
+  <si>
+    <t>KMHintCollapsed</t>
+  </si>
+  <si>
+    <t>按&lt;b&gt;回车&lt;/b&gt;继续</t>
+  </si>
+  <si>
+    <t>KMHintExtend</t>
+  </si>
+  <si>
+    <t>按&lt;b&gt;[回车]&lt;/b&gt;继续</t>
+  </si>
+  <si>
+    <t>NextTutorial</t>
+  </si>
+  <si>
+    <t>下一教程</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>PlayLevel</t>
+  </si>
+  <si>
+    <t>游玩关卡</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>ReleaseToReturn_KM</t>
+  </si>
+  <si>
+    <t>松开以返回</t>
+  </si>
+  <si>
+    <t>Release to Hide</t>
+  </si>
+  <si>
+    <t>Restart</t>
+  </si>
+  <si>
+    <t>重新开始</t>
+  </si>
+  <si>
+    <t>StartGame</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;开始游戏&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Start Game&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>TouchHintCollapsed</t>
+  </si>
+  <si>
+    <t>点&lt;b&gt;这里&lt;/b&gt;继续</t>
+  </si>
+  <si>
+    <t>TouchHintExtend</t>
+  </si>
+  <si>
+    <t>点&lt;b&gt;[这里]&lt;/b&gt;继续</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;新手指南&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Tutorial&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>TutorialBasicControl</t>
+  </si>
+  <si>
+    <t>TutorialDestroyer</t>
+  </si>
+  <si>
+    <t>TutorialGoalAndCycle</t>
+  </si>
+  <si>
+    <t>TutorialSectionOver</t>
+  </si>
+  <si>
+    <t>此段教程结束</t>
+  </si>
+  <si>
+    <t>Section Over</t>
+  </si>
+  <si>
+    <t>TutorialShop</t>
+  </si>
+  <si>
+    <t>TutorialSignalBasic</t>
+  </si>
+  <si>
+    <t>Level_1</t>
+  </si>
+  <si>
+    <t>第一关</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level_2</t>
+  </si>
+  <si>
+    <t>第二关</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level_3</t>
+  </si>
+  <si>
+    <t>第三关</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level_4</t>
+  </si>
+  <si>
+    <t>第四关</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level_5</t>
+  </si>
+  <si>
+    <t>第五关</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>TutorialShop_Currency</t>
+  </si>
+  <si>
+    <t>TutorialSignalBasic_Adv</t>
+  </si>
+  <si>
+    <t>第一天上班</t>
+  </si>
+  <si>
+    <t>First Day to Work</t>
+  </si>
+  <si>
+    <t>用点儿脑子</t>
+  </si>
+  <si>
+    <t>Use your Brain</t>
+  </si>
+  <si>
+    <t>时间不等人</t>
+  </si>
+  <si>
+    <t>Time awaits</t>
+  </si>
+  <si>
+    <t>买买买</t>
+  </si>
+  <si>
+    <t>Shut up and TMM</t>
+  </si>
+  <si>
+    <t>别瞎花钱</t>
+  </si>
+  <si>
+    <t>Watch your wallet</t>
+  </si>
+  <si>
+    <t>来点儿别的</t>
+  </si>
+  <si>
+    <t>Some new trick</t>
+  </si>
+  <si>
+    <t>搁一起呢？</t>
+  </si>
+  <si>
+    <t>Put it all together</t>
+  </si>
+  <si>
+    <t>别太放松</t>
+  </si>
+  <si>
+    <t>Heads Up!</t>
+  </si>
+  <si>
+    <t>TutorialGoal</t>
+  </si>
+  <si>
+    <t>Need to do:</t>
+  </si>
+  <si>
+    <t>任务目标:</t>
+  </si>
+  <si>
+    <t>TutorialTimeAdv</t>
+  </si>
+  <si>
+    <t>该干活了</t>
+  </si>
+  <si>
+    <t>Time to work</t>
+  </si>
+  <si>
+    <t>TutorialComplexSignal</t>
+  </si>
+  <si>
+    <t>EndingMessageTutorialFailed</t>
+  </si>
+  <si>
+    <t>本节教程未完成</t>
+  </si>
+  <si>
+    <t>This section of tutorial is not finished</t>
+  </si>
+  <si>
+    <t>NextTutorialFailed</t>
+  </si>
+  <si>
+    <t>再试一下</t>
+  </si>
+  <si>
+    <t>Retry</t>
+  </si>
+  <si>
+    <t>返回主菜单的按钮名称</t>
+  </si>
+  <si>
+    <t>游戏内容显示的操作提示（键盘版）</t>
+  </si>
+  <si>
+    <t>游戏内容显示的操作提示（触屏版）</t>
+  </si>
+  <si>
+    <t>开始生涯模式按钮名称</t>
+  </si>
+  <si>
+    <t>游戏结束时，显示的内容</t>
+  </si>
+  <si>
+    <t>按"回车"以返回</t>
+  </si>
+  <si>
+    <t>按"回车"以完成任务</t>
+  </si>
+  <si>
+    <t>Press "Enter" to Return</t>
+  </si>
+  <si>
+    <t>Press "Enter" to Complete</t>
+  </si>
+  <si>
+    <t>KMEnterToReturn</t>
+  </si>
+  <si>
+    <t>KMEnterToComplete</t>
+  </si>
+  <si>
+    <t>TouchToReturn</t>
+  </si>
+  <si>
+    <t>TouchToComplete</t>
+  </si>
+  <si>
+    <t>按这里以返回</t>
+  </si>
+  <si>
+    <t>按这里以完成任务</t>
+  </si>
+  <si>
+    <t>Touch HERE to Complete</t>
+  </si>
+  <si>
+    <t>Touch HERE to Return</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>AdvShop_KM</t>
+  </si>
+  <si>
+    <t>AdvShop_2_KM</t>
+  </si>
+  <si>
+    <t>AdvShop_Touch</t>
+  </si>
+  <si>
+    <t>AdvShop_2_Touch</t>
+  </si>
+  <si>
+    <t>左Alt取消购买</t>
+  </si>
+  <si>
+    <t>按这里取消购买</t>
+  </si>
+  <si>
+    <t>右Shift:随机位置——（+0元)
+回车键:光标位置 ——（+{[VALUE]}元）</t>
+  </si>
+  <si>
+    <t>按这里:随机位置——（+0元)
+点击棋盘位置:棋盘位置 ——（+{[VALUE]}元）</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">【方向键】：移动光标
 【方向键】+【空格】：拖动单元
 【左Shift】：旋转单元
-【TAB】：查看数据范围</t>
+【TAB】：查看数据范围
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>【</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>点击左Ctrl】：可强制演进一步。</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>【滑动单元】：拖动单元
+【双击单元】：旋转单元
+【双指按住】：查看数据范围
+【按住屏幕中空白位置】：可强制演进一步。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>&lt;b&gt;[Arrows]:&lt;/b&gt; Move Cursor
 &lt;b&gt;[Arrows+SpaceBar]:&lt;/b&gt; Drag Unit
 &lt;b&gt;[Left-Shift]:&lt;/b&gt; Rotate Unit
-&lt;b&gt;[TAB]:&lt;/b&gt; Visualize Signal</t>
-  </si>
-  <si>
-    <t>BasicControl_Touch</t>
-  </si>
-  <si>
-    <t>【滑动单元】：拖动单元
-【双击单元】：旋转单元
-【双指按住】：查看数据范围</t>
+&lt;b&gt;[TAB]:&lt;/b&gt; Visualize Signal
+&lt;b&gt;[Left Ctrl]:&lt;/b&gt; Force to move to next round</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>&lt;b&gt;[Swipe on Unit]:&lt;/b&gt;Drag Unit
 &lt;b&gt;[DoubleTap on Unit]:&lt;/b&gt;Rotate Unit
-&lt;b&gt;[DoubleFinger Hold]:&lt;/b&gt;Visualize Signal</t>
-  </si>
-  <si>
-    <t>CareerButton</t>
-  </si>
-  <si>
-    <t>生涯模式</t>
-  </si>
-  <si>
-    <t>Career</t>
-  </si>
-  <si>
-    <t>EndingMessageNormal_EarnedMoney</t>
-  </si>
-  <si>
-    <t>时间到了，你赚了{[VALUE]}块钱[i2p_Zero]时间到了，但你没赚钱</t>
-  </si>
-  <si>
-    <t>Time Up, and you earned {[VALUE]} money[i2p_Zero]Time Up, and you earned no money</t>
-  </si>
-  <si>
-    <t>EndingMessageNormal_NoEarnedMoney</t>
-  </si>
-  <si>
-    <t>时间到了，你赔了{[VALUE]}块钱[i2p_Zero]时间到了，但你也没赔钱</t>
-  </si>
-  <si>
-    <t>Time Up, and you lost {[VALUE]} money[i2p_Zero]Time Up, but you haven't lost money</t>
-  </si>
-  <si>
-    <t>EndingMessageNormal_NoMoney</t>
-  </si>
-  <si>
-    <t>你没钱了！</t>
-  </si>
-  <si>
-    <t>You've run out of money.</t>
-  </si>
-  <si>
-    <t>EndingMessageTutorial</t>
-  </si>
-  <si>
-    <t>本节教程结束~</t>
-  </si>
-  <si>
-    <t>This section of tutorial has concluded</t>
-  </si>
-  <si>
-    <t>GameOver</t>
-  </si>
-  <si>
-    <t>游戏结束</t>
-  </si>
-  <si>
-    <t>GAME OVER</t>
-  </si>
-  <si>
-    <t>HForHint_KM</t>
-  </si>
-  <si>
-    <t>按住&lt;b&gt;[H]&lt;/b&gt;键查看操作说明</t>
-  </si>
-  <si>
-    <t>Hold &lt;b&gt;[H]&lt;/b&gt; for controlling</t>
-  </si>
-  <si>
-    <t>HForHint_Touch</t>
-  </si>
-  <si>
-    <t>按住这里查看操作说明</t>
-  </si>
-  <si>
-    <t>Hold Here for Hint</t>
-  </si>
-  <si>
-    <t>KMHintCollapsed</t>
-  </si>
-  <si>
-    <t>按&lt;b&gt;回车&lt;/b&gt;继续</t>
-  </si>
-  <si>
-    <t>KMHintExtend</t>
-  </si>
-  <si>
-    <t>按&lt;b&gt;[回车]&lt;/b&gt;继续</t>
-  </si>
-  <si>
-    <t>NextTutorial</t>
-  </si>
-  <si>
-    <t>下一教程</t>
-  </si>
-  <si>
-    <t>Next</t>
-  </si>
-  <si>
-    <t>PlayLevel</t>
-  </si>
-  <si>
-    <t>游玩关卡</t>
-  </si>
-  <si>
-    <t>Play</t>
-  </si>
-  <si>
-    <t>ReleaseToReturn_KM</t>
-  </si>
-  <si>
-    <t>松开以返回</t>
-  </si>
-  <si>
-    <t>Release to Hide</t>
-  </si>
-  <si>
-    <t>Restart</t>
-  </si>
-  <si>
-    <t>重新开始</t>
-  </si>
-  <si>
-    <t>StartGame</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;开始游戏&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Start Game&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>TouchHintCollapsed</t>
-  </si>
-  <si>
-    <t>点&lt;b&gt;这里&lt;/b&gt;继续</t>
-  </si>
-  <si>
-    <t>TouchHintExtend</t>
-  </si>
-  <si>
-    <t>点&lt;b&gt;[这里]&lt;/b&gt;继续</t>
-  </si>
-  <si>
-    <t>Tutorial</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;新手指南&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Tutorial&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>TutorialBasicControl</t>
-  </si>
-  <si>
-    <t>TutorialDestroyer</t>
-  </si>
-  <si>
-    <t>TutorialGoalAndCycle</t>
-  </si>
-  <si>
-    <t>TutorialSectionOver</t>
-  </si>
-  <si>
-    <t>此段教程结束</t>
-  </si>
-  <si>
-    <t>Section Over</t>
-  </si>
-  <si>
-    <t>TutorialShop</t>
-  </si>
-  <si>
-    <t>TutorialSignalBasic</t>
-  </si>
-  <si>
-    <t>Level_1</t>
-  </si>
-  <si>
-    <t>第一关</t>
-  </si>
-  <si>
-    <t>Level 1</t>
-  </si>
-  <si>
-    <t>Level_2</t>
-  </si>
-  <si>
-    <t>第二关</t>
-  </si>
-  <si>
-    <t>Level 2</t>
-  </si>
-  <si>
-    <t>Level_3</t>
-  </si>
-  <si>
-    <t>第三关</t>
-  </si>
-  <si>
-    <t>Level 3</t>
-  </si>
-  <si>
-    <t>Level_4</t>
-  </si>
-  <si>
-    <t>第四关</t>
-  </si>
-  <si>
-    <t>Level 4</t>
-  </si>
-  <si>
-    <t>Level_5</t>
-  </si>
-  <si>
-    <t>第五关</t>
-  </si>
-  <si>
-    <t>Level 5</t>
-  </si>
-  <si>
-    <t>TutorialShop_Currency</t>
-  </si>
-  <si>
-    <t>TutorialSignalBasic_Adv</t>
-  </si>
-  <si>
-    <t>第一天上班</t>
-  </si>
-  <si>
-    <t>First Day to Work</t>
-  </si>
-  <si>
-    <t>用点儿脑子</t>
-  </si>
-  <si>
-    <t>Use your Brain</t>
-  </si>
-  <si>
-    <t>时间不等人</t>
-  </si>
-  <si>
-    <t>Time awaits</t>
-  </si>
-  <si>
-    <t>买买买</t>
-  </si>
-  <si>
-    <t>Shut up and TMM</t>
-  </si>
-  <si>
-    <t>别瞎花钱</t>
-  </si>
-  <si>
-    <t>Watch your wallet</t>
-  </si>
-  <si>
-    <t>来点儿别的</t>
-  </si>
-  <si>
-    <t>Some new trick</t>
-  </si>
-  <si>
-    <t>搁一起呢？</t>
-  </si>
-  <si>
-    <t>Put it all together</t>
-  </si>
-  <si>
-    <t>别太放松</t>
-  </si>
-  <si>
-    <t>Heads Up!</t>
-  </si>
-  <si>
-    <t>TutorialGoal</t>
-  </si>
-  <si>
-    <t>Need to do:</t>
-  </si>
-  <si>
-    <t>任务目标:</t>
-  </si>
-  <si>
-    <t>TutorialTimeAdv</t>
-  </si>
-  <si>
-    <t>该干活了</t>
-  </si>
-  <si>
-    <t>Time to work</t>
-  </si>
-  <si>
-    <t>TutorialComplexSignal</t>
-  </si>
-  <si>
-    <t>EndingMessageTutorialFailed</t>
-  </si>
-  <si>
-    <t>本节教程未完成</t>
-  </si>
-  <si>
-    <t>This section of tutorial is not finished</t>
-  </si>
-  <si>
-    <t>NextTutorialFailed</t>
-  </si>
-  <si>
-    <t>再试一下</t>
-  </si>
-  <si>
-    <t>Retry</t>
-  </si>
-  <si>
-    <t>返回主菜单的按钮名称</t>
-  </si>
-  <si>
-    <t>游戏内容显示的操作提示（键盘版）</t>
-  </si>
-  <si>
-    <t>游戏内容显示的操作提示（触屏版）</t>
-  </si>
-  <si>
-    <t>开始生涯模式按钮名称</t>
-  </si>
-  <si>
-    <t>游戏结束时，显示的内容</t>
-  </si>
-  <si>
-    <t>按"回车"以返回</t>
-  </si>
-  <si>
-    <t>按"回车"以完成任务</t>
-  </si>
-  <si>
-    <t>Press "Enter" to Return</t>
-  </si>
-  <si>
-    <t>Press "Enter" to Complete</t>
-  </si>
-  <si>
-    <t>KMEnterToReturn</t>
-  </si>
-  <si>
-    <t>KMEnterToComplete</t>
-  </si>
-  <si>
-    <t>TouchToReturn</t>
-  </si>
-  <si>
-    <t>TouchToComplete</t>
-  </si>
-  <si>
-    <t>按这里以返回</t>
-  </si>
-  <si>
-    <t>按这里以完成任务</t>
-  </si>
-  <si>
-    <t>Touch HERE to Complete</t>
-  </si>
-  <si>
-    <t>Touch HERE to Return</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>AdvShop_KM</t>
-  </si>
-  <si>
-    <t>AdvShop_2_KM</t>
-  </si>
-  <si>
-    <t>AdvShop_Touch</t>
-  </si>
-  <si>
-    <t>AdvShop_2_Touch</t>
-  </si>
-  <si>
-    <t>左Alt取消购买</t>
-  </si>
-  <si>
-    <t>按这里取消购买</t>
-  </si>
-  <si>
-    <t>右Shift:随机位置——（+0元)
-回车键:光标位置 ——（+{[VALUE]}元）</t>
-  </si>
-  <si>
-    <t>按这里:随机位置——（+0元)
-点击棋盘位置:棋盘位置 ——（+{[VALUE]}元）</t>
+&lt;b&gt;[DoubleFinger Hold]:&lt;/b&gt;Visualize Signal
+&lt;b&gt;[Hold on Empty spot]:&lt;/b&gt;Force to move to next round</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -479,7 +510,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -487,7 +518,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -496,7 +527,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -505,7 +536,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -514,7 +545,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -522,7 +553,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -530,7 +561,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -538,7 +569,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -546,7 +577,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -555,7 +586,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -564,7 +595,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -572,7 +603,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -581,7 +612,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -589,7 +620,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -598,7 +629,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -607,7 +638,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -615,9 +646,23 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -993,30 +1038,30 @@
     <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1330,18 +1375,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="2" customWidth="1"/>
-    <col min="4" max="4" width="44.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.1796875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="44.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1361,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1369,7 +1414,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -1378,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58">
+    <row r="3" spans="1:5" ht="70">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1386,661 +1431,663 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="70">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.5">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="42">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="29">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="42">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.5">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="28">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="28">
+      <c r="A45" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="29">
-      <c r="A45" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="B45" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>